<commit_message>
Item compression, sorting changes, refactorings
</commit_message>
<xml_diff>
--- a/packages/ambre/tests/actual_expected/rule_extraction_wikipedia_consequent_bread.expected.xlsx
+++ b/packages/ambre/tests/actual_expected/rule_extraction_wikipedia_consequent_bread.expected.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,22 +50,21 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -474,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>milk</t>
+          <t>butter</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,16 +482,16 @@
         </is>
       </c>
       <c r="C2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>1.666666666666667</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2</v>
-      </c>
       <c r="F2" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -501,7 +500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>butter</t>
+          <t>milk</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -510,22 +509,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8333333333333334</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>